<commit_message>
Write data into excel file after reading data from excel file
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -32,8 +32,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -64,8 +65,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,38 +399,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
-        <v>name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>code</v>
+      <c r="A1" s="1" t="str">
+        <v>Stockcode</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <v>Product Class</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <v>Stock UOM</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <v>Warehouse</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <v>Supplier</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <v>List Price</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <v>Unit Cost</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <v>Product Category</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>test</v>
-      </c>
-      <c r="B2" t="str">
-        <v>102</v>
+      <c r="A2" s="1">
+        <v>26012504000</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <v>MURRPLASTIK MP 26125, R 40, LP</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <v>MU01</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <v>EA</v>
+      </c>
+      <c r="E2" s="1">
+        <v>90</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <v>INNO002</v>
+      </c>
+      <c r="G2" s="1">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <v>M</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
-        <v>test1</v>
-      </c>
-      <c r="B3" t="str">
-        <v>103</v>
+      <c r="A3" s="1">
+        <v>46012504001</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <v>MANUALLY ADDED ITEMS</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <v>AB01</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <v>EA</v>
+      </c>
+      <c r="E3" s="1">
+        <v>90</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <v>INNO002</v>
+      </c>
+      <c r="G3" s="1">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1">
+        <v>21</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <v>M</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="str">
+        <v>12343-000</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <v>OMRON WSHR PLT OC J1 HRMNC DRV</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <v>OM09</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <v>EA</v>
+      </c>
+      <c r="E4" s="1">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <v>INNO002</v>
+      </c>
+      <c r="G4" s="1">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <v>M</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>